<commit_message>
change number of digit
</commit_message>
<xml_diff>
--- a/Graph for Simple Multiplication.xlsx
+++ b/Graph for Simple Multiplication.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danis\Desktop\CPT 212\CPT212-Asg1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEDDE14-A1CD-4CC6-A37C-EC9CB2950B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859F3E3F-B6D3-492B-91EF-706A52026DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{318B4E69-23ED-4155-91B1-FEDFF76B5611}"/>
   </bookViews>
@@ -155,14 +155,18 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Number</a:t>
+              <a:rPr lang="en-MY"/>
+              <a:t>Number of Operations against n</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> of Operations against n</a:t>
+              <a:rPr lang="en-MY"/>
+              <a:t>Simple Multiplication</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -202,10 +206,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11921716595009482"/>
-          <c:y val="0.10965262379896527"/>
-          <c:w val="0.79184637229299681"/>
-          <c:h val="0.76226461542655111"/>
+          <c:x val="0.13667894902484953"/>
+          <c:y val="0.13535808023997001"/>
+          <c:w val="0.79584717247854697"/>
+          <c:h val="0.77467918433272764"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -394,7 +398,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FE6B-4947-A2DF-BD2AE43D456C}"/>
+              <c16:uniqueId val="{00000000-4675-4EFA-8D5A-F125B667DBFC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -407,11 +411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="321932464"/>
-        <c:axId val="321932944"/>
+        <c:axId val="52380704"/>
+        <c:axId val="52392224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="321932464"/>
+        <c:axId val="52380704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -457,14 +461,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.46616857551896923"/>
-              <c:y val="0.92113506761110819"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -495,7 +491,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -531,12 +527,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321932944"/>
+        <c:crossAx val="52392224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="321932944"/>
+        <c:axId val="52392224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321932464"/>
+        <c:crossAx val="52380704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -685,6 +681,576 @@
     <a:p>
       <a:pPr>
         <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY"/>
+              <a:t>Number of Operations against n</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-MY"/>
+              <a:t>Simple Multiplication</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13667894902484953"/>
+          <c:y val="0.13535808023997001"/>
+          <c:w val="0.79584717247854697"/>
+          <c:h val="0.77467918433272764"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Number of Operations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="l"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>185.03229999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>313.10340000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>478.3295</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>680.7645</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>920.87599999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1196.116</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1510.7489</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1859.5001999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2247.0542999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2672.7910000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4675-4EFA-8D5A-F125B667DBFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="l"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="52380704"/>
+        <c:axId val="52392224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="52380704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52392224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="52392224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-MY"/>
+                  <a:t>Average Number of Operations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52380704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr b="0" i="0" baseline="0"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -737,7 +1303,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1258,15 +2380,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>415</xdr:colOff>
+      <xdr:colOff>416</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>174764</xdr:rowOff>
+      <xdr:rowOff>182384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>401707</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>174764</xdr:rowOff>
+      <xdr:colOff>132523</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1286,6 +2408,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>416</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>18637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>136333</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C34C8E3-47A3-41E3-67EC-34B98F986C61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1593,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94FC801D-002F-47E6-8D45-6527CD336ABB}">
   <dimension ref="B3:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="92" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="C14" sqref="B3:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>